<commit_message>
A few notes and changes when adding data to neo4j
</commit_message>
<xml_diff>
--- a/Porter/data.xlsx
+++ b/Porter/data.xlsx
@@ -6437,7 +6437,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6460,10 +6460,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -6494,7 +6490,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31524,7 +31520,7 @@
       </c>
     </row>
     <row r="639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A639" s="6" t="s">
+      <c r="A639" s="3" t="s">
         <v>1549</v>
       </c>
       <c r="C639" s="0" t="s">
@@ -31550,7 +31546,7 @@
       </c>
     </row>
     <row r="640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A640" s="6" t="s">
+      <c r="A640" s="3" t="s">
         <v>1551</v>
       </c>
       <c r="C640" s="0" t="s">
@@ -31583,12 +31579,12 @@
       <c r="U640" s="1" t="s">
         <v>1547</v>
       </c>
-      <c r="V640" s="6" t="s">
+      <c r="V640" s="3" t="s">
         <v>1549</v>
       </c>
     </row>
     <row r="641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A641" s="6" t="s">
+      <c r="A641" s="3" t="s">
         <v>1553</v>
       </c>
       <c r="C641" s="0" t="s">
@@ -31621,7 +31617,7 @@
       <c r="U641" s="1" t="s">
         <v>1547</v>
       </c>
-      <c r="V641" s="6" t="s">
+      <c r="V641" s="3" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -31746,7 +31742,7 @@
       </c>
     </row>
     <row r="645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A645" s="6" t="s">
+      <c r="A645" s="3" t="s">
         <v>1562</v>
       </c>
       <c r="C645" s="0" t="s">
@@ -31769,7 +31765,7 @@
       </c>
     </row>
     <row r="646" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A646" s="6" t="s">
+      <c r="A646" s="3" t="s">
         <v>1564</v>
       </c>
       <c r="C646" s="0" t="s">
@@ -31807,7 +31803,7 @@
       </c>
     </row>
     <row r="647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A647" s="6" t="s">
+      <c r="A647" s="3" t="s">
         <v>1566</v>
       </c>
       <c r="C647" s="0" t="s">
@@ -31845,7 +31841,7 @@
       </c>
     </row>
     <row r="648" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A648" s="6" t="s">
+      <c r="A648" s="3" t="s">
         <v>1568</v>
       </c>
       <c r="C648" s="0" t="s">
@@ -31927,7 +31923,7 @@
       </c>
     </row>
     <row r="650" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A650" s="6" t="s">
+      <c r="A650" s="3" t="s">
         <v>1572</v>
       </c>
       <c r="C650" s="0" t="s">
@@ -31950,7 +31946,7 @@
       </c>
     </row>
     <row r="651" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A651" s="6" t="s">
+      <c r="A651" s="3" t="s">
         <v>1574</v>
       </c>
       <c r="C651" s="0" t="s">
@@ -31988,7 +31984,7 @@
       </c>
     </row>
     <row r="652" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A652" s="6" t="s">
+      <c r="A652" s="3" t="s">
         <v>1575</v>
       </c>
       <c r="C652" s="0" t="s">
@@ -32178,7 +32174,7 @@
       </c>
     </row>
     <row r="657" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A657" s="6" t="s">
+      <c r="A657" s="3" t="s">
         <v>1583</v>
       </c>
       <c r="C657" s="0" t="s">
@@ -36708,7 +36704,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="7" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="6" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -36925,7 +36921,7 @@
       <c r="H8" s="0" t="s">
         <v>1806</v>
       </c>
-      <c r="I8" s="7" t="n">
+      <c r="I8" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -36998,7 +36994,7 @@
       <c r="H11" s="0" t="s">
         <v>1811</v>
       </c>
-      <c r="I11" s="7" t="n">
+      <c r="I11" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -37106,7 +37102,7 @@
       <c r="H15" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="I15" s="7" t="n">
+      <c r="I15" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -37568,7 +37564,7 @@
       <c r="H40" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="I40" s="7" t="n">
+      <c r="I40" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -37601,7 +37597,7 @@
       <c r="H41" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="I41" s="7" t="n">
+      <c r="I41" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -37769,7 +37765,7 @@
       <c r="G48" s="0" t="n">
         <v>1981</v>
       </c>
-      <c r="I48" s="7" t="n">
+      <c r="I48" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -38447,7 +38443,7 @@
       <c r="H76" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="I76" s="7" t="n">
+      <c r="I76" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -38474,7 +38470,7 @@
       <c r="G77" s="0" t="n">
         <v>1962</v>
       </c>
-      <c r="I77" s="7" t="n">
+      <c r="I77" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -38544,7 +38540,7 @@
       <c r="G80" s="0" t="n">
         <v>1970</v>
       </c>
-      <c r="I80" s="7" t="n">
+      <c r="I80" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -38649,7 +38645,7 @@
       <c r="H84" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="I84" s="7" t="n">
+      <c r="I84" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -38762,7 +38758,7 @@
       <c r="H89" s="0" t="s">
         <v>717</v>
       </c>
-      <c r="I89" s="7" t="n">
+      <c r="I89" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -38919,7 +38915,7 @@
       <c r="H95" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="I95" s="7" t="n">
+      <c r="I95" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -38966,7 +38962,7 @@
       <c r="H97" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="I97" s="7" t="n">
+      <c r="I97" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -38987,7 +38983,7 @@
       <c r="G98" s="0" t="n">
         <v>1966</v>
       </c>
-      <c r="I98" s="7" t="n">
+      <c r="I98" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -39144,7 +39140,7 @@
       <c r="H104" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="I104" s="7" t="n">
+      <c r="I104" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -39272,7 +39268,7 @@
       <c r="G109" s="0" t="n">
         <v>1967</v>
       </c>
-      <c r="I109" s="7" t="n">
+      <c r="I109" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -39296,7 +39292,7 @@
       <c r="G110" s="0" t="n">
         <v>1975</v>
       </c>
-      <c r="I110" s="7" t="n">
+      <c r="I110" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -39704,7 +39700,7 @@
       <c r="H126" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="I126" s="7" t="n">
+      <c r="I126" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -39864,7 +39860,7 @@
       <c r="H132" s="0" t="s">
         <v>1948</v>
       </c>
-      <c r="I132" s="7" t="n">
+      <c r="I132" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -39925,7 +39921,7 @@
       <c r="G135" s="0" t="n">
         <v>1973</v>
       </c>
-      <c r="I135" s="7" t="n">
+      <c r="I135" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -39952,7 +39948,7 @@
       <c r="G136" s="0" t="n">
         <v>1977</v>
       </c>
-      <c r="I136" s="7" t="n">
+      <c r="I136" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -40013,7 +40009,7 @@
       <c r="G139" s="0" t="n">
         <v>1976</v>
       </c>
-      <c r="I139" s="7" t="n">
+      <c r="I139" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -40138,7 +40134,7 @@
       <c r="G144" s="0" t="n">
         <v>1981</v>
       </c>
-      <c r="I144" s="7" t="n">
+      <c r="I144" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -40165,7 +40161,7 @@
       <c r="G145" s="0" t="n">
         <v>1981</v>
       </c>
-      <c r="I145" s="7" t="n">
+      <c r="I145" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -40244,7 +40240,7 @@
       <c r="H148" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="I148" s="7" t="n">
+      <c r="I148" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -40430,7 +40426,7 @@
       <c r="G155" s="0" t="n">
         <v>1966</v>
       </c>
-      <c r="I155" s="7" t="n">
+      <c r="I155" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -40460,7 +40456,7 @@
       <c r="H156" s="0" t="s">
         <v>1204</v>
       </c>
-      <c r="I156" s="7" t="n">
+      <c r="I156" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -40593,7 +40589,7 @@
       <c r="D162" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I162" s="7" t="n">
+      <c r="I162" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -40787,7 +40783,8 @@
       <c r="H170" s="0" t="s">
         <v>1297</v>
       </c>
-      <c r="I170" s="7" t="b">
+      <c r="I170" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -41454,7 +41451,8 @@
       <c r="H199" s="0" t="s">
         <v>2035</v>
       </c>
-      <c r="I199" s="7" t="b">
+      <c r="I199" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="L199" s="0" t="n">
@@ -41486,7 +41484,8 @@
       <c r="H200" s="0" t="s">
         <v>2035</v>
       </c>
-      <c r="I200" s="7" t="b">
+      <c r="I200" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="L200" s="0" t="n">
@@ -41518,7 +41517,8 @@
       <c r="H201" s="0" t="s">
         <v>2038</v>
       </c>
-      <c r="I201" s="7" t="b">
+      <c r="I201" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="L201" s="0" t="n">
@@ -41668,7 +41668,8 @@
       <c r="H207" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="I207" s="7" t="b">
+      <c r="I207" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="J207" s="0" t="s">
@@ -41815,7 +41816,8 @@
       <c r="H213" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="I213" s="7" t="b">
+      <c r="I213" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="L213" s="0" t="n">
@@ -42029,7 +42031,8 @@
       <c r="H221" s="0" t="s">
         <v>2062</v>
       </c>
-      <c r="I221" s="7" t="b">
+      <c r="I221" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="L221" s="0" t="n">
@@ -42263,7 +42266,8 @@
       <c r="H230" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="I230" s="7" t="b">
+      <c r="I230" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="L230" s="0" t="n">

</xml_diff>